<commit_message>
Added additional fuel inventories
</commit_message>
<xml_diff>
--- a/rmnd_lca/data/additional_inventories/lci-hydrogen-coal-gasification.xlsx
+++ b/rmnd_lca/data/additional_inventories/lci-hydrogen-coal-gasification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romai\Documents\GitHub\rmnd-lca\rmnd_lca\data\additional_inventories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C06EE59D-C0E2-4BA8-B76D-3DC34EC549B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED5D2E35-BF29-4556-A80C-B7A8A3D980BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -603,7 +603,7 @@
   <dimension ref="A1:J301"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Issue in hydrogen inventory
</commit_message>
<xml_diff>
--- a/rmnd_lca/data/additional_inventories/lci-hydrogen-coal-gasification.xlsx
+++ b/rmnd_lca/data/additional_inventories/lci-hydrogen-coal-gasification.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romai\Documents\GitHub\rmnd-lca\rmnd_lca\data\additional_inventories\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sacchi_r\Documents\GitHub\rmnd-lca\rmnd_lca\data\additional_inventories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED5D2E35-BF29-4556-A80C-B7A8A3D980BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="25815" windowHeight="14025"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1274" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1274" uniqueCount="76">
   <si>
     <t>Activity</t>
   </si>
@@ -258,12 +257,15 @@
   </si>
   <si>
     <t>Hydrogen from coal Gasification</t>
+  </si>
+  <si>
+    <t>Hydrogen, gaseous, 30 bar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -599,21 +601,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J301"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A263" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I286" sqref="I286"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.453125" customWidth="1"/>
-    <col min="5" max="5" width="47.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.42578125" customWidth="1"/>
+    <col min="5" max="5" width="47.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>51</v>
       </c>
@@ -621,7 +623,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -629,7 +631,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -637,15 +639,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -653,7 +655,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -661,7 +663,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -669,7 +671,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -677,7 +679,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>56</v>
       </c>
@@ -685,12 +687,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -722,7 +724,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -748,7 +750,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -774,7 +776,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -800,7 +802,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>54</v>
       </c>
@@ -820,10 +822,10 @@
         <v>22</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -852,7 +854,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -881,7 +883,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -910,7 +912,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -936,7 +938,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -965,7 +967,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>71</v>
       </c>
@@ -994,7 +996,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>45</v>
       </c>
@@ -1023,7 +1025,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -1052,7 +1054,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>49</v>
       </c>
@@ -1081,7 +1083,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>52</v>
       </c>
@@ -1110,7 +1112,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>0</v>
       </c>
@@ -1118,7 +1120,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>1</v>
       </c>
@@ -1126,15 +1128,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>2</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>3</v>
       </c>
@@ -1142,7 +1144,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -1150,7 +1152,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -1158,7 +1160,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>13</v>
       </c>
@@ -1166,7 +1168,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>56</v>
       </c>
@@ -1174,12 +1176,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>7</v>
       </c>
@@ -1211,7 +1213,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>14</v>
       </c>
@@ -1237,7 +1239,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>19</v>
       </c>
@@ -1263,7 +1265,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>20</v>
       </c>
@@ -1289,7 +1291,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>54</v>
       </c>
@@ -1309,10 +1311,10 @@
         <v>22</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>23</v>
       </c>
@@ -1341,7 +1343,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>28</v>
       </c>
@@ -1370,7 +1372,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>31</v>
       </c>
@@ -1399,7 +1401,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>34</v>
       </c>
@@ -1425,7 +1427,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>36</v>
       </c>
@@ -1454,7 +1456,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>71</v>
       </c>
@@ -1483,7 +1485,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>45</v>
       </c>
@@ -1512,7 +1514,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>46</v>
       </c>
@@ -1541,7 +1543,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -1570,7 +1572,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>52</v>
       </c>
@@ -1599,7 +1601,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>0</v>
       </c>
@@ -1607,7 +1609,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>1</v>
       </c>
@@ -1615,15 +1617,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>2</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>3</v>
       </c>
@@ -1631,7 +1633,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>5</v>
       </c>
@@ -1639,7 +1641,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>9</v>
       </c>
@@ -1647,7 +1649,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>13</v>
       </c>
@@ -1655,7 +1657,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>56</v>
       </c>
@@ -1663,12 +1665,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>7</v>
       </c>
@@ -1700,7 +1702,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>14</v>
       </c>
@@ -1726,7 +1728,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>19</v>
       </c>
@@ -1752,7 +1754,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>20</v>
       </c>
@@ -1778,7 +1780,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>54</v>
       </c>
@@ -1798,10 +1800,10 @@
         <v>22</v>
       </c>
       <c r="J66" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>23</v>
       </c>
@@ -1830,7 +1832,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>28</v>
       </c>
@@ -1859,7 +1861,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>31</v>
       </c>
@@ -1888,7 +1890,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>34</v>
       </c>
@@ -1914,7 +1916,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>36</v>
       </c>
@@ -1943,7 +1945,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>40</v>
       </c>
@@ -1972,7 +1974,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>45</v>
       </c>
@@ -2001,7 +2003,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>46</v>
       </c>
@@ -2030,7 +2032,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>49</v>
       </c>
@@ -2059,7 +2061,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>52</v>
       </c>
@@ -2088,7 +2090,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>0</v>
       </c>
@@ -2096,7 +2098,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>1</v>
       </c>
@@ -2104,15 +2106,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>2</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>3</v>
       </c>
@@ -2120,7 +2122,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>5</v>
       </c>
@@ -2128,7 +2130,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>9</v>
       </c>
@@ -2136,7 +2138,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>13</v>
       </c>
@@ -2144,7 +2146,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>56</v>
       </c>
@@ -2152,12 +2154,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>7</v>
       </c>
@@ -2189,7 +2191,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>14</v>
       </c>
@@ -2215,7 +2217,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>19</v>
       </c>
@@ -2241,7 +2243,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>20</v>
       </c>
@@ -2267,7 +2269,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>54</v>
       </c>
@@ -2287,10 +2289,10 @@
         <v>22</v>
       </c>
       <c r="J91" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>23</v>
       </c>
@@ -2319,7 +2321,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>28</v>
       </c>
@@ -2348,7 +2350,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>31</v>
       </c>
@@ -2377,7 +2379,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>34</v>
       </c>
@@ -2403,7 +2405,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>36</v>
       </c>
@@ -2432,7 +2434,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>40</v>
       </c>
@@ -2461,7 +2463,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>45</v>
       </c>
@@ -2490,7 +2492,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>46</v>
       </c>
@@ -2519,7 +2521,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>49</v>
       </c>
@@ -2548,7 +2550,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>52</v>
       </c>
@@ -2577,7 +2579,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="103" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>0</v>
       </c>
@@ -2585,7 +2587,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>1</v>
       </c>
@@ -2593,15 +2595,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>2</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>3</v>
       </c>
@@ -2609,7 +2611,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>5</v>
       </c>
@@ -2617,7 +2619,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>9</v>
       </c>
@@ -2625,7 +2627,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>13</v>
       </c>
@@ -2633,7 +2635,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>56</v>
       </c>
@@ -2641,12 +2643,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="111" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>7</v>
       </c>
@@ -2678,7 +2680,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>14</v>
       </c>
@@ -2704,7 +2706,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>19</v>
       </c>
@@ -2730,7 +2732,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>20</v>
       </c>
@@ -2756,7 +2758,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="116" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>54</v>
       </c>
@@ -2776,10 +2778,10 @@
         <v>22</v>
       </c>
       <c r="J116" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>23</v>
       </c>
@@ -2808,7 +2810,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>28</v>
       </c>
@@ -2837,7 +2839,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>31</v>
       </c>
@@ -2866,7 +2868,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>34</v>
       </c>
@@ -2892,7 +2894,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>36</v>
       </c>
@@ -2921,7 +2923,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>40</v>
       </c>
@@ -2950,7 +2952,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>45</v>
       </c>
@@ -2979,7 +2981,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>46</v>
       </c>
@@ -3008,7 +3010,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>49</v>
       </c>
@@ -3037,7 +3039,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>52</v>
       </c>
@@ -3066,7 +3068,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="128" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>0</v>
       </c>
@@ -3074,7 +3076,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>1</v>
       </c>
@@ -3082,15 +3084,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>2</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>3</v>
       </c>
@@ -3098,7 +3100,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>5</v>
       </c>
@@ -3106,7 +3108,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>9</v>
       </c>
@@ -3114,7 +3116,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>13</v>
       </c>
@@ -3122,7 +3124,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>56</v>
       </c>
@@ -3130,12 +3132,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="136" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>7</v>
       </c>
@@ -3167,7 +3169,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>14</v>
       </c>
@@ -3193,7 +3195,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>19</v>
       </c>
@@ -3219,7 +3221,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>20</v>
       </c>
@@ -3245,7 +3247,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="141" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>54</v>
       </c>
@@ -3265,10 +3267,10 @@
         <v>22</v>
       </c>
       <c r="J141" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>23</v>
       </c>
@@ -3297,7 +3299,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>28</v>
       </c>
@@ -3326,7 +3328,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>31</v>
       </c>
@@ -3355,7 +3357,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>34</v>
       </c>
@@ -3381,7 +3383,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>36</v>
       </c>
@@ -3410,7 +3412,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>40</v>
       </c>
@@ -3439,7 +3441,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>45</v>
       </c>
@@ -3468,7 +3470,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>46</v>
       </c>
@@ -3497,7 +3499,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>49</v>
       </c>
@@ -3526,7 +3528,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>52</v>
       </c>
@@ -3555,7 +3557,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="153" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>0</v>
       </c>
@@ -3563,7 +3565,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>1</v>
       </c>
@@ -3571,15 +3573,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>2</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>3</v>
       </c>
@@ -3587,7 +3589,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>5</v>
       </c>
@@ -3595,7 +3597,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>9</v>
       </c>
@@ -3603,7 +3605,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>13</v>
       </c>
@@ -3611,7 +3613,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>56</v>
       </c>
@@ -3619,12 +3621,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="161" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>7</v>
       </c>
@@ -3656,7 +3658,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>14</v>
       </c>
@@ -3682,7 +3684,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>19</v>
       </c>
@@ -3708,7 +3710,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>20</v>
       </c>
@@ -3734,7 +3736,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="166" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>54</v>
       </c>
@@ -3754,10 +3756,10 @@
         <v>22</v>
       </c>
       <c r="J166" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>23</v>
       </c>
@@ -3786,7 +3788,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>28</v>
       </c>
@@ -3815,7 +3817,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>31</v>
       </c>
@@ -3844,7 +3846,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>34</v>
       </c>
@@ -3870,7 +3872,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>36</v>
       </c>
@@ -3899,7 +3901,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>40</v>
       </c>
@@ -3928,7 +3930,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>45</v>
       </c>
@@ -3957,7 +3959,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>46</v>
       </c>
@@ -3986,7 +3988,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>49</v>
       </c>
@@ -4015,7 +4017,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>52</v>
       </c>
@@ -4044,7 +4046,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="178" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>0</v>
       </c>
@@ -4052,7 +4054,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>1</v>
       </c>
@@ -4060,15 +4062,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>2</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>3</v>
       </c>
@@ -4076,7 +4078,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>5</v>
       </c>
@@ -4084,7 +4086,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>9</v>
       </c>
@@ -4092,7 +4094,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>13</v>
       </c>
@@ -4100,7 +4102,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>56</v>
       </c>
@@ -4108,12 +4110,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="186" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>7</v>
       </c>
@@ -4145,7 +4147,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>14</v>
       </c>
@@ -4171,7 +4173,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>19</v>
       </c>
@@ -4197,7 +4199,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>20</v>
       </c>
@@ -4223,7 +4225,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="191" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
         <v>54</v>
       </c>
@@ -4243,10 +4245,10 @@
         <v>22</v>
       </c>
       <c r="J191" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>23</v>
       </c>
@@ -4275,7 +4277,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>28</v>
       </c>
@@ -4304,7 +4306,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>31</v>
       </c>
@@ -4333,7 +4335,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>34</v>
       </c>
@@ -4359,7 +4361,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>36</v>
       </c>
@@ -4388,7 +4390,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>40</v>
       </c>
@@ -4417,7 +4419,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>45</v>
       </c>
@@ -4446,7 +4448,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>46</v>
       </c>
@@ -4475,7 +4477,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>49</v>
       </c>
@@ -4504,7 +4506,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>52</v>
       </c>
@@ -4533,7 +4535,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="203" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>0</v>
       </c>
@@ -4541,7 +4543,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>1</v>
       </c>
@@ -4549,15 +4551,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>2</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>3</v>
       </c>
@@ -4565,7 +4567,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>5</v>
       </c>
@@ -4573,7 +4575,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>9</v>
       </c>
@@ -4581,7 +4583,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>13</v>
       </c>
@@ -4589,7 +4591,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>56</v>
       </c>
@@ -4597,12 +4599,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="211" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>7</v>
       </c>
@@ -4634,7 +4636,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>14</v>
       </c>
@@ -4660,7 +4662,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>19</v>
       </c>
@@ -4686,7 +4688,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>20</v>
       </c>
@@ -4712,7 +4714,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="216" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
         <v>54</v>
       </c>
@@ -4732,10 +4734,10 @@
         <v>22</v>
       </c>
       <c r="J216" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>23</v>
       </c>
@@ -4764,7 +4766,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>28</v>
       </c>
@@ -4793,7 +4795,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>31</v>
       </c>
@@ -4822,7 +4824,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>34</v>
       </c>
@@ -4848,7 +4850,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>36</v>
       </c>
@@ -4877,7 +4879,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>40</v>
       </c>
@@ -4906,7 +4908,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>45</v>
       </c>
@@ -4935,7 +4937,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>46</v>
       </c>
@@ -4964,7 +4966,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>49</v>
       </c>
@@ -4993,7 +4995,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>52</v>
       </c>
@@ -5022,7 +5024,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="228" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>0</v>
       </c>
@@ -5030,7 +5032,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>1</v>
       </c>
@@ -5038,15 +5040,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>2</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>3</v>
       </c>
@@ -5054,7 +5056,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>5</v>
       </c>
@@ -5062,7 +5064,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>9</v>
       </c>
@@ -5070,7 +5072,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>13</v>
       </c>
@@ -5078,7 +5080,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>56</v>
       </c>
@@ -5086,12 +5088,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="236" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>7</v>
       </c>
@@ -5123,7 +5125,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>14</v>
       </c>
@@ -5149,7 +5151,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>19</v>
       </c>
@@ -5175,7 +5177,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>20</v>
       </c>
@@ -5201,7 +5203,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="241" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A241" s="2" t="s">
         <v>54</v>
       </c>
@@ -5221,10 +5223,10 @@
         <v>22</v>
       </c>
       <c r="J241" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>23</v>
       </c>
@@ -5253,7 +5255,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>28</v>
       </c>
@@ -5282,7 +5284,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>31</v>
       </c>
@@ -5311,7 +5313,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>34</v>
       </c>
@@ -5337,7 +5339,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>36</v>
       </c>
@@ -5366,7 +5368,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>40</v>
       </c>
@@ -5395,7 +5397,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>45</v>
       </c>
@@ -5424,7 +5426,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>46</v>
       </c>
@@ -5453,7 +5455,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>49</v>
       </c>
@@ -5482,7 +5484,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>52</v>
       </c>
@@ -5511,7 +5513,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="253" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
         <v>0</v>
       </c>
@@ -5519,7 +5521,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>1</v>
       </c>
@@ -5527,15 +5529,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="255" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>2</v>
       </c>
       <c r="B255" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>3</v>
       </c>
@@ -5543,7 +5545,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>5</v>
       </c>
@@ -5551,7 +5553,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>9</v>
       </c>
@@ -5559,7 +5561,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>13</v>
       </c>
@@ -5567,7 +5569,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>56</v>
       </c>
@@ -5575,12 +5577,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="261" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>7</v>
       </c>
@@ -5612,7 +5614,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>14</v>
       </c>
@@ -5638,7 +5640,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>19</v>
       </c>
@@ -5664,7 +5666,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>20</v>
       </c>
@@ -5690,7 +5692,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="266" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A266" s="2" t="s">
         <v>54</v>
       </c>
@@ -5710,10 +5712,10 @@
         <v>22</v>
       </c>
       <c r="J266" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>23</v>
       </c>
@@ -5742,7 +5744,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>28</v>
       </c>
@@ -5771,7 +5773,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>31</v>
       </c>
@@ -5800,7 +5802,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>34</v>
       </c>
@@ -5826,7 +5828,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>36</v>
       </c>
@@ -5855,7 +5857,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>40</v>
       </c>
@@ -5884,7 +5886,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="273" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>45</v>
       </c>
@@ -5913,7 +5915,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="274" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>46</v>
       </c>
@@ -5942,7 +5944,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="275" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>49</v>
       </c>
@@ -5971,7 +5973,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="276" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>52</v>
       </c>
@@ -6000,7 +6002,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="278" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
         <v>0</v>
       </c>
@@ -6008,7 +6010,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="279" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>1</v>
       </c>
@@ -6016,15 +6018,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="280" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>2</v>
       </c>
       <c r="B280" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="281" spans="1:10" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>3</v>
       </c>
@@ -6032,7 +6034,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="282" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>5</v>
       </c>
@@ -6040,7 +6042,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="283" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>9</v>
       </c>
@@ -6048,7 +6050,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="284" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>13</v>
       </c>
@@ -6056,7 +6058,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="285" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>56</v>
       </c>
@@ -6064,12 +6066,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="286" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="287" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>7</v>
       </c>
@@ -6101,7 +6103,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="288" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>14</v>
       </c>
@@ -6127,7 +6129,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="289" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>19</v>
       </c>
@@ -6153,7 +6155,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="290" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>20</v>
       </c>
@@ -6179,7 +6181,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="291" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A291" s="2" t="s">
         <v>54</v>
       </c>
@@ -6199,10 +6201,10 @@
         <v>22</v>
       </c>
       <c r="J291" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="292" spans="1:10" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="292" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>23</v>
       </c>
@@ -6231,7 +6233,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="293" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>28</v>
       </c>
@@ -6260,7 +6262,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="294" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>31</v>
       </c>
@@ -6289,7 +6291,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="295" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>34</v>
       </c>
@@ -6315,7 +6317,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="296" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>36</v>
       </c>
@@ -6344,7 +6346,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="297" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>40</v>
       </c>
@@ -6373,7 +6375,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="298" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>45</v>
       </c>
@@ -6402,7 +6404,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="299" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>46</v>
       </c>
@@ -6431,7 +6433,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="300" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>49</v>
       </c>
@@ -6460,7 +6462,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="301" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>52</v>
       </c>

</xml_diff>